<commit_message>
Final clean up of Scott' branch before merging with master
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="16100" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="nextflow.config" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
   <si>
     <t>//</t>
   </si>
@@ -263,6 +263,63 @@
   </si>
   <si>
     <t>queue</t>
+  </si>
+  <si>
+    <t>#AWS options</t>
+  </si>
+  <si>
+    <t>AWS access key (confidential)</t>
+  </si>
+  <si>
+    <t>AWS secret key (very confidential)</t>
+  </si>
+  <si>
+    <t>accessKey</t>
+  </si>
+  <si>
+    <t>secretKey</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>AWS region</t>
+  </si>
+  <si>
+    <t>AWS AMI to be used</t>
+  </si>
+  <si>
+    <t>ami-9dc5a68a</t>
+  </si>
+  <si>
+    <t>AMI</t>
+  </si>
+  <si>
+    <t>AWS instance type</t>
+  </si>
+  <si>
+    <t>instanceType</t>
+  </si>
+  <si>
+    <t>subnet-8ee22c7</t>
+  </si>
+  <si>
+    <t>bootStorageSize</t>
+  </si>
+  <si>
+    <t>How big boot image should be</t>
+  </si>
+  <si>
+    <t>20GB</t>
+  </si>
+  <si>
+    <t>AWS maximum number of instances to be used</t>
+  </si>
+  <si>
+    <t>maxInstances</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -677,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -988,6 +1045,79 @@
         <v>56</v>
       </c>
     </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
updated Java config generator
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16100" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="10100" yWindow="640" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="nextflow.config" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="99">
   <si>
     <t>//</t>
   </si>
@@ -301,9 +301,6 @@
     <t>instanceType</t>
   </si>
   <si>
-    <t>subnet-8ee22c7</t>
-  </si>
-  <si>
     <t>bootStorageSize</t>
   </si>
   <si>
@@ -320,6 +317,30 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>Image with LaTeX installed</t>
+  </si>
+  <si>
+    <t>latexImage</t>
+  </si>
+  <si>
+    <t>m4.xlarge</t>
+  </si>
+  <si>
+    <t>AWS EFS/sharedStorage ID</t>
+  </si>
+  <si>
+    <t>sharedStorage</t>
+  </si>
+  <si>
+    <t>Mount of Amazon EFS/sharedStorage</t>
+  </si>
+  <si>
+    <t>sharedStorageMount</t>
+  </si>
+  <si>
+    <t>/mnt/shared</t>
   </si>
 </sst>
 </file>
@@ -387,8 +408,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -400,11 +423,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -734,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1047,75 +1072,102 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" t="s">
         <v>89</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C35" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>91</v>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the xlsx file and the config-java har
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="640" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31280" windowHeight="21380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="nextflow.config" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <author>Scott</author>
   </authors>
   <commentList>
-    <comment ref="A13" authorId="0">
+    <comment ref="A14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>//</t>
   </si>
@@ -73,6 +73,9 @@
     <t>${params.work_dir}/scripts</t>
   </si>
   <si>
+    <t>data_name</t>
+  </si>
+  <si>
     <t>high_ld_regions_fname</t>
   </si>
   <si>
@@ -115,12 +118,18 @@
     <t>max_plink_cores</t>
   </si>
   <si>
+    <t>process.queue</t>
+  </si>
+  <si>
     <t>Directory in which the Nextflow scripts can be found</t>
   </si>
   <si>
     <t>Where output should go?</t>
   </si>
   <si>
+    <t>Name of the input data file</t>
+  </si>
+  <si>
     <t>Do we have sex information?</t>
   </si>
   <si>
@@ -142,6 +151,9 @@
     <t>User specified value</t>
   </si>
   <si>
+    <t>raw-GWA-data</t>
+  </si>
+  <si>
     <t>high_LD_regions_37.ssv</t>
   </si>
   <si>
@@ -208,15 +220,9 @@
     <t>plinkImage</t>
   </si>
   <si>
-    <t>banshee1221/h3agwas-plink</t>
-  </si>
-  <si>
     <t>Image with R installed</t>
   </si>
   <si>
-    <t>banshee1221/h3agwas-r</t>
-  </si>
-  <si>
     <t>rEngineImage</t>
   </si>
   <si>
@@ -262,85 +268,19 @@
     <t>YRI</t>
   </si>
   <si>
-    <t>queue</t>
-  </si>
-  <si>
-    <t>#AWS options</t>
-  </si>
-  <si>
-    <t>AWS access key (confidential)</t>
-  </si>
-  <si>
-    <t>AWS secret key (very confidential)</t>
-  </si>
-  <si>
-    <t>accessKey</t>
-  </si>
-  <si>
-    <t>secretKey</t>
-  </si>
-  <si>
-    <t>region</t>
-  </si>
-  <si>
-    <t>AWS region</t>
-  </si>
-  <si>
-    <t>AWS AMI to be used</t>
-  </si>
-  <si>
-    <t>ami-9dc5a68a</t>
-  </si>
-  <si>
-    <t>AMI</t>
-  </si>
-  <si>
-    <t>AWS instance type</t>
-  </si>
-  <si>
-    <t>instanceType</t>
-  </si>
-  <si>
-    <t>bootStorageSize</t>
-  </si>
-  <si>
-    <t>How big boot image should be</t>
-  </si>
-  <si>
-    <t>20GB</t>
-  </si>
-  <si>
-    <t>AWS maximum number of instances to be used</t>
-  </si>
-  <si>
-    <t>maxInstances</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Image with LaTeX installed</t>
-  </si>
-  <si>
-    <t>latexImage</t>
-  </si>
-  <si>
-    <t>m4.xlarge</t>
-  </si>
-  <si>
-    <t>AWS EFS/sharedStorage ID</t>
-  </si>
-  <si>
-    <t>sharedStorage</t>
-  </si>
-  <si>
-    <t>Mount of Amazon EFS/sharedStorage</t>
-  </si>
-  <si>
-    <t>sharedStorageMount</t>
-  </si>
-  <si>
-    <t>/mnt/shared</t>
+    <t>Image with TexLive</t>
+  </si>
+  <si>
+    <t>texliveImage</t>
+  </si>
+  <si>
+    <t>h3abionet_org/h3agwas-texlive</t>
+  </si>
+  <si>
+    <t>h3abionet_org/h3agwas-plink</t>
+  </si>
+  <si>
+    <t>h3abionet_org/h3agwas-rtools</t>
   </si>
 </sst>
 </file>
@@ -379,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,12 +329,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,28 +342,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -759,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -777,25 +706,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G1"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -806,8 +735,8 @@
       <c r="G2"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
-        <v>67</v>
+      <c r="A3" t="s">
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -818,23 +747,23 @@
       <c r="G3"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>68</v>
+      <c r="A4" t="s">
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="3" t="s">
-        <v>24</v>
+      <c r="A5" t="s">
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -846,7 +775,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -858,7 +787,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -866,35 +795,32 @@
       <c r="G7"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>26</v>
+      <c r="A8" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
-        <v>32</v>
+      <c r="C8" t="s">
+        <v>35</v>
       </c>
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>59</v>
+      <c r="D9" t="s">
+        <v>36</v>
       </c>
       <c r="G9"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -902,16 +828,20 @@
       <c r="C10" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -922,252 +852,174 @@
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>66</v>
+      <c r="C22" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" t="s">
-        <v>49</v>
+        <v>23</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
         <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
         <v>74</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>94</v>
-      </c>
-      <c r="B36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the config-gen file
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13140" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1600" yWindow="2180" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="nextflow.config" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="137">
   <si>
     <t>//</t>
   </si>
@@ -52,6 +52,9 @@
     <t>work_dir</t>
   </si>
   <si>
+    <t>/$HOME/h3agwas</t>
+  </si>
+  <si>
     <t>input_dir</t>
   </si>
   <si>
@@ -193,39 +196,12 @@
     <t>#QC options</t>
   </si>
   <si>
-    <t>long</t>
-  </si>
-  <si>
     <t>Queue (name of queue that should be used IF job scheduler used, ignored otherwise)</t>
   </si>
   <si>
-    <t>#Docker options -- IGNORED if docker not used</t>
-  </si>
-  <si>
-    <t>Image with PLINK installed</t>
-  </si>
-  <si>
-    <t>plinkImage</t>
-  </si>
-  <si>
-    <t>Image with R installed</t>
-  </si>
-  <si>
-    <t>rEngineImage</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
     <t>0.343</t>
   </si>
   <si>
-    <t>0.254</t>
-  </si>
-  <si>
     <t>0.05</t>
   </si>
   <si>
@@ -253,184 +229,232 @@
     <t>*</t>
   </si>
   <si>
-    <t>Image with TexLive</t>
-  </si>
-  <si>
-    <t>h3abionet_org/h3agwas-texlive</t>
-  </si>
-  <si>
-    <t>h3abionet_org/h3agwas-plink</t>
-  </si>
-  <si>
-    <t>latexImage</t>
-  </si>
-  <si>
     <t>#Options only needed if converting from Illumina TOP/BOT</t>
   </si>
   <si>
-    <t>Are we using top/bot as input</t>
-  </si>
-  <si>
-    <t>topbot</t>
-  </si>
-  <si>
     <t>false</t>
   </si>
   <si>
     <t>true</t>
   </si>
   <si>
-    <t xml:space="preserve">Fam file -- provide a fam file in PLINK format </t>
-  </si>
-  <si>
-    <t>fam</t>
+    <t>Illumina Chip Manifest</t>
+  </si>
+  <si>
+    <t>/data/aux/HumanOmni5-4-v1-0-D.csv</t>
+  </si>
+  <si>
+    <t>manifest</t>
+  </si>
+  <si>
+    <t>#Config options</t>
+  </si>
+  <si>
+    <t>#Options for Amazon EC2</t>
+  </si>
+  <si>
+    <t>AMI</t>
+  </si>
+  <si>
+    <t>accessKey</t>
+  </si>
+  <si>
+    <t>secretKey</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>instanceType</t>
+  </si>
+  <si>
+    <t>bootStorageSize</t>
+  </si>
+  <si>
+    <t>maxInstances</t>
+  </si>
+  <si>
+    <t>ID of the Amazon AM to be used</t>
+  </si>
+  <si>
+    <t>Your access key</t>
+  </si>
+  <si>
+    <t>Your secret key</t>
+  </si>
+  <si>
+    <t>Region to execute in</t>
+  </si>
+  <si>
+    <t>Instance type</t>
+  </si>
+  <si>
+    <t>Storage for boot</t>
+  </si>
+  <si>
+    <t>sharedStorageID</t>
+  </si>
+  <si>
+    <t>Global storage for cluster (EFS)</t>
+  </si>
+  <si>
+    <t>How many instances</t>
+  </si>
+  <si>
+    <t>20GB</t>
+  </si>
+  <si>
+    <t>sharedStorageMount</t>
+  </si>
+  <si>
+    <t>/mnt/shared</t>
+  </si>
+  <si>
+    <t>Directory on Amazon cluster where scripts and data are</t>
+  </si>
+  <si>
+    <t>subnetID</t>
+  </si>
+  <si>
+    <t>ID of the Amazon subnet on which your cluster runs</t>
+  </si>
+  <si>
+    <t>m4.xlarge</t>
+  </si>
+  <si>
+    <t>eu-west-1</t>
+  </si>
+  <si>
+    <t>ami-9ca7b2fa</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>sampleA</t>
+  </si>
+  <si>
+    <t>Chip description (can be same as manifest or has column with physical coordinates)</t>
+  </si>
+  <si>
+    <t>chipdescription</t>
+  </si>
+  <si>
+    <t>/external/diskA/novartis/metadata/HumanOmni5-4v1_B_Physical-and-Genetic-Coordinates.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strandreport </t>
+  </si>
+  <si>
+    <t>strandreport</t>
+  </si>
+  <si>
+    <t>0.150</t>
+  </si>
+  <si>
+    <t>Batch report</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>Batch column</t>
+  </si>
+  <si>
+    <t>batch_col</t>
+  </si>
+  <si>
+    <t>For doing batch QC</t>
+  </si>
+  <si>
+    <t>phenotype</t>
+  </si>
+  <si>
+    <t>Phenotype file (optional for batch analysis)</t>
+  </si>
+  <si>
+    <t>Phenotype column</t>
+  </si>
+  <si>
+    <t>pheno_col</t>
+  </si>
+  <si>
+    <t>if phenotype is false, doesn't matter</t>
+  </si>
+  <si>
+    <t>Case-control file</t>
+  </si>
+  <si>
+    <t>case_control</t>
+  </si>
+  <si>
+    <t>data.phe</t>
+  </si>
+  <si>
+    <t>Case-control column</t>
+  </si>
+  <si>
+    <t>case_control_col</t>
+  </si>
+  <si>
+    <t>pheno</t>
+  </si>
+  <si>
+    <t>String -- name of column (plink mpheno file). Ignored if case_control above is empty</t>
+  </si>
+  <si>
+    <t>if batch is empty, doesn't matter</t>
+  </si>
+  <si>
+    <t>If batch is empty, doesn’'t matter</t>
+  </si>
+  <si>
+    <t>Can use manifest</t>
+  </si>
+  <si>
+    <t>Output alignment (against which strand? Illumnia, dbSNP or reference)</t>
+  </si>
+  <si>
+    <t>output_align</t>
+  </si>
+  <si>
+    <t>topbottom</t>
+  </si>
+  <si>
+    <t>dbsnp or ref</t>
   </si>
   <si>
     <t>reference</t>
   </si>
   <si>
-    <t>Reference genome for your chip</t>
-  </si>
-  <si>
-    <t>/data/aux/Homo_sapiens.GRCh37.75.dna.toplevel.fa</t>
-  </si>
-  <si>
-    <t>SNP Merge table from NCBI (ftp.ncbi.nlm.nih.gov/snp/organisms/human_9606/database)</t>
-  </si>
-  <si>
-    <t>/data/aux/RsMergeArch.bcp.gz</t>
-  </si>
-  <si>
-    <t>vcf_merge_table</t>
-  </si>
-  <si>
-    <t>dbSNP list</t>
-  </si>
-  <si>
-    <t>/data/aux/All_20170403.vcf.gz</t>
-  </si>
-  <si>
-    <t>Illumina Chip Manifest</t>
-  </si>
-  <si>
-    <t>/data/aux/HumanOmni5-4-v1-0-D.csv</t>
-  </si>
-  <si>
-    <t>manifest</t>
-  </si>
-  <si>
-    <t>#Config options</t>
-  </si>
-  <si>
-    <t>BioPerl image</t>
-  </si>
-  <si>
-    <t>bioperlImage</t>
-  </si>
-  <si>
-    <t>bioperl/bioperl</t>
-  </si>
-  <si>
-    <t>Image with gemma installed</t>
-  </si>
-  <si>
-    <t>gemmaImage</t>
-  </si>
-  <si>
-    <t>h3abionet_org/h3agwas-gemma</t>
-  </si>
-  <si>
-    <t>dbsnp_all_vcf</t>
-  </si>
-  <si>
-    <t>#Options for Amazon EC2</t>
-  </si>
-  <si>
-    <t>AMI</t>
-  </si>
-  <si>
-    <t>accessKey</t>
-  </si>
-  <si>
-    <t>secretKey</t>
-  </si>
-  <si>
-    <t>region</t>
-  </si>
-  <si>
-    <t>instanceType</t>
-  </si>
-  <si>
-    <t>bootStorageSize</t>
-  </si>
-  <si>
-    <t>maxInstances</t>
-  </si>
-  <si>
-    <t>ID of the Amazon AM to be used</t>
-  </si>
-  <si>
-    <t>Your access key</t>
-  </si>
-  <si>
-    <t>Your secret key</t>
-  </si>
-  <si>
-    <t>Region to execute in</t>
-  </si>
-  <si>
-    <t>Instance type</t>
-  </si>
-  <si>
-    <t>Storage for boot</t>
-  </si>
-  <si>
-    <t>sharedStorageID</t>
-  </si>
-  <si>
-    <t>Global storage for cluster (EFS)</t>
-  </si>
-  <si>
-    <t>How many instances</t>
-  </si>
-  <si>
-    <t>20GB</t>
-  </si>
-  <si>
-    <t>sharedStorageMount</t>
-  </si>
-  <si>
-    <t>/mnt/shared</t>
-  </si>
-  <si>
-    <t>Directory on Amazon cluster where scripts and data are</t>
-  </si>
-  <si>
-    <t>subnetID</t>
-  </si>
-  <si>
-    <t>ID of the Amazon subnet on which your cluster runs</t>
-  </si>
-  <si>
-    <t>m4.xlarge</t>
-  </si>
-  <si>
-    <t>eu-west-1</t>
-  </si>
-  <si>
-    <t>ami-9ca7b2fa</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>sampleA</t>
-  </si>
-  <si>
-    <t>h3abionet_org/h3agwas-r</t>
-  </si>
-  <si>
-    <t>/$PWD</t>
+    <t>h3a37.ref</t>
+  </si>
+  <si>
+    <t>samplesheet</t>
+  </si>
+  <si>
+    <t>/data/aux/H3Africa_2017_20021485_A3_StrandReport_FDT.txt</t>
+  </si>
+  <si>
+    <t>Reference genome (entry for each position in chip)</t>
+  </si>
+  <si>
+    <t>/data/experiment/samples.xlx</t>
+  </si>
+  <si>
+    <t>Sample sheet (entry for each person)</t>
+  </si>
+  <si>
+    <t>Try to abbreviate participant IDs from sample sheet</t>
+  </si>
+  <si>
+    <t>abbrev</t>
+  </si>
+  <si>
+    <t>Which file has case_control info</t>
+  </si>
+  <si>
+    <t>site</t>
   </si>
 </sst>
 </file>
@@ -498,8 +522,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -515,15 +551,27 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -853,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -871,88 +919,88 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G1"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G5"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -961,415 +1009,484 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G9"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G19"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E24"/>
+      <c r="F24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="3" t="s">
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="2" t="s">
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="2" t="s">
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" t="s">
         <v>86</v>
       </c>
-      <c r="B35" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="B48" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>107</v>
-      </c>
-      <c r="B38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>108</v>
-      </c>
-      <c r="B39" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>109</v>
-      </c>
-      <c r="B40" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>110</v>
-      </c>
-      <c r="B41" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>111</v>
-      </c>
-      <c r="B42" t="s">
-        <v>104</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>115</v>
-      </c>
-      <c r="B44" t="s">
-        <v>106</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>114</v>
-      </c>
-      <c r="B45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>119</v>
-      </c>
-      <c r="B46" t="s">
-        <v>117</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>121</v>
-      </c>
-      <c r="B47" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>